<commit_message>
format nursing home data
</commit_message>
<xml_diff>
--- a/data/deaths_location.xlsx
+++ b/data/deaths_location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan\Documents\GitHub\International-COVID-IFR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB986F1-BA30-4D99-8F50-CAABC87891D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77F9FBC-6B2D-4FDD-9604-A2097E743948}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="1050" windowWidth="9930" windowHeight="9150" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
+    <workbookView xWindow="8480" yWindow="2900" windowWidth="9930" windowHeight="9150" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>country</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Canada</t>
   </si>
   <si>
-    <t>news reports state 79% of covid deaths attributed to care homes</t>
-  </si>
-  <si>
     <t>Germany</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>https://www.thestar.com/politics/federal/2020/05/07/82-of-canadas-covid-19-deaths-have-been-in-long-term-care.html</t>
   </si>
 </sst>
 </file>
@@ -514,14 +514,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0957DDB2-FF5A-4350-800D-AA3314930578}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.36328125" customWidth="1"/>
     <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -676,9 +678,8 @@
       <c r="C6">
         <v>1375</v>
       </c>
-      <c r="D6">
-        <f>550+66</f>
-        <v>616</v>
+      <c r="E6">
+        <v>857</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>15</v>
@@ -690,6 +691,9 @@
       </c>
       <c r="B7" s="1">
         <v>43965</v>
+      </c>
+      <c r="C7">
+        <v>2899</v>
       </c>
       <c r="E7">
         <v>1637</v>
@@ -729,7 +733,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1">
         <v>43943</v>
@@ -741,12 +745,12 @@
         <v>1599</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1">
         <v>43945</v>
@@ -758,16 +762,24 @@
         <v>133</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1">
+        <v>43957</v>
+      </c>
+      <c r="C11">
+        <v>4167</v>
+      </c>
+      <c r="E11">
+        <v>3436</v>
+      </c>
       <c r="I11" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -785,6 +797,7 @@
     <hyperlink ref="I8" r:id="rId7" xr:uid="{E6D2BBE8-183F-4497-9029-7DBB5687D6D3}"/>
     <hyperlink ref="I9" r:id="rId8" display="https://www.springermedizin.de/covid-19/infektionserkrankungen-in-der-hausarztpraxis/ein-drittel-aller-covid-19-todesfaelle-in-heimen/17924978" xr:uid="{C3939348-4E7A-4FF8-8317-F3A901DD03D3}"/>
     <hyperlink ref="I10" r:id="rId9" xr:uid="{552A9600-AAD6-462A-9E96-6A6C246201B3}"/>
+    <hyperlink ref="I11" r:id="rId10" xr:uid="{80DEF0DD-2E38-4B48-913C-4EF68FE67545}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -792,15 +805,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92843AD0-5FB3-42F6-BF08-1FFA91F45A80}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -820,10 +836,13 @@
         <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -846,8 +865,11 @@
         <f>SUM(E2:F2)</f>
         <v>160</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -870,8 +892,11 @@
         <f t="shared" ref="G3:G9" si="0">SUM(E3:F3)</f>
         <v>277</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -894,8 +919,11 @@
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -918,8 +946,11 @@
         <f t="shared" si="0"/>
         <v>717</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -942,8 +973,11 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -966,8 +1000,11 @@
         <f t="shared" si="0"/>
         <v>166</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -990,8 +1027,11 @@
         <f t="shared" si="0"/>
         <v>288</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1014,13 +1054,16 @@
         <f t="shared" si="0"/>
         <v>856</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>70</v>
@@ -1040,13 +1083,16 @@
         <f>G2+G6</f>
         <v>245</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11">
         <v>75</v>
@@ -1066,13 +1112,16 @@
         <f t="shared" si="1"/>
         <v>443</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>80</v>
@@ -1092,13 +1141,16 @@
         <f t="shared" si="1"/>
         <v>638</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13">
         <v>85</v>
@@ -1117,6 +1169,9 @@
       <c r="G13">
         <f t="shared" si="1"/>
         <v>1573</v>
+      </c>
+      <c r="H13" s="1">
+        <v>43965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add adjusted death data for 4 countries
</commit_message>
<xml_diff>
--- a/data/deaths_location.xlsx
+++ b/data/deaths_location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan\Documents\GitHub\International-COVID-IFR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BCC0D1-7D79-428C-A25D-6A2892E02DC2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E698192E-64E4-4A47-8498-7AB054D9D590}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
+    <workbookView xWindow="7520" yWindow="1210" windowWidth="13640" windowHeight="9170" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
   <si>
     <t>country</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Germany</t>
   </si>
   <si>
-    <t>https://www.springermedizin.de/covid-19/infektionserkrankungen-in-der-hausarztpraxis/ein-drittel-aller-covid-19-todesfaelle-in-heimen/17924978  https://ltccovid.org/wp-content/uploads/2020/04/Germany_LTC_COVID-19-23-April-2020_updated.pdf</t>
-  </si>
-  <si>
     <t>Denmark</t>
   </si>
   <si>
@@ -155,6 +152,30 @@
   </si>
   <si>
     <t>01/05/02020</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>https://interaktiv.tagesanzeiger.ch/2020/corona-tote-mehrheitlich-aus-altersheimen/</t>
+  </si>
+  <si>
+    <t>Geneva</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>https://ltccovid.org/wp-content/uploads/2020/05/Mortality-associated-with-COVID-3-May-final-6.pdf</t>
+  </si>
+  <si>
+    <t>pLTC</t>
   </si>
 </sst>
 </file>
@@ -518,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0957DDB2-FF5A-4350-800D-AA3314930578}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,7 +553,7 @@
     <col min="5" max="5" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -558,13 +579,16 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -586,11 +610,15 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2">
+        <f>E2/C2</f>
+        <v>0.44755680049797697</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -616,11 +644,15 @@
       <c r="H3">
         <v>127</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3">
+        <f t="shared" ref="I3:I17" si="0">E3/C3</f>
+        <v>0.26056581804449758</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -646,16 +678,20 @@
       <c r="H4">
         <v>3</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0.26372924648786716</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="C5">
         <f>31777+1566</f>
@@ -680,11 +716,15 @@
       <c r="H5">
         <v>130</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.26071439282608044</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -704,11 +744,15 @@
       <c r="F6">
         <v>31</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.45742904841402338</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -721,11 +765,15 @@
       <c r="E7">
         <v>857</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0.62327272727272731</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -738,14 +786,18 @@
       <c r="E8">
         <v>1637</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0.56467747499137633</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -767,30 +819,38 @@
       <c r="H9">
         <v>36</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0.51005302695536903</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="1">
-        <v>43943</v>
+        <v>43954</v>
       </c>
       <c r="C10">
-        <v>4879</v>
+        <v>6649</v>
       </c>
       <c r="E10">
-        <v>1599</v>
-      </c>
-      <c r="I10" s="2" t="s">
+        <v>2401</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0.36110693337343963</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>34</v>
       </c>
       <c r="B11" s="1">
         <v>43945</v>
@@ -801,11 +861,15 @@
       <c r="E11">
         <v>133</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0.33756345177664976</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -818,26 +882,136 @@
       <c r="E12">
         <v>3436</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="1"/>
-      <c r="I13" s="2"/>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.82457403407727381</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43963</v>
+      </c>
+      <c r="C13">
+        <v>1749</v>
+      </c>
+      <c r="E13">
+        <v>927</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.53001715265866212</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43963</v>
+      </c>
+      <c r="C14">
+        <v>154</v>
+      </c>
+      <c r="E14">
+        <v>109</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.70779220779220775</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="1">
+        <v>43939</v>
+      </c>
+      <c r="C15">
+        <v>172</v>
+      </c>
+      <c r="E15">
+        <v>33</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0.19186046511627908</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1">
+        <v>43953</v>
+      </c>
+      <c r="C16">
+        <v>211</v>
+      </c>
+      <c r="E16">
+        <v>127</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0.6018957345971564</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1">
+        <v>43944</v>
+      </c>
+      <c r="C17">
+        <v>820</v>
+      </c>
+      <c r="E17">
+        <v>327</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0.39878048780487807</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I6" r:id="rId1" xr:uid="{C202A423-D2AD-48A5-81D8-FD47A34E7068}"/>
-    <hyperlink ref="I7" r:id="rId2" xr:uid="{FFD58B59-920D-4BB1-984F-DCE9EBAD12A8}"/>
-    <hyperlink ref="I2" r:id="rId3" xr:uid="{F4DD4505-BDBA-4F91-9F18-D97C282F5BDA}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{0DFB8553-11C3-4C67-B11F-12F0B2E880D1}"/>
-    <hyperlink ref="I4" r:id="rId5" xr:uid="{15BF439D-4123-4A54-9B3D-42B9C4A470E3}"/>
-    <hyperlink ref="I8" r:id="rId6" xr:uid="{83C09D43-1C91-4DE0-AEBF-986F38CE3FF5}"/>
-    <hyperlink ref="I9" r:id="rId7" xr:uid="{E6D2BBE8-183F-4497-9029-7DBB5687D6D3}"/>
-    <hyperlink ref="I10" r:id="rId8" display="https://www.springermedizin.de/covid-19/infektionserkrankungen-in-der-hausarztpraxis/ein-drittel-aller-covid-19-todesfaelle-in-heimen/17924978" xr:uid="{C3939348-4E7A-4FF8-8317-F3A901DD03D3}"/>
-    <hyperlink ref="I11" r:id="rId9" xr:uid="{552A9600-AAD6-462A-9E96-6A6C246201B3}"/>
-    <hyperlink ref="I12" r:id="rId10" xr:uid="{80DEF0DD-2E38-4B48-913C-4EF68FE67545}"/>
+    <hyperlink ref="J6" r:id="rId1" xr:uid="{C202A423-D2AD-48A5-81D8-FD47A34E7068}"/>
+    <hyperlink ref="J7" r:id="rId2" xr:uid="{FFD58B59-920D-4BB1-984F-DCE9EBAD12A8}"/>
+    <hyperlink ref="J2" r:id="rId3" xr:uid="{F4DD4505-BDBA-4F91-9F18-D97C282F5BDA}"/>
+    <hyperlink ref="J3" r:id="rId4" xr:uid="{0DFB8553-11C3-4C67-B11F-12F0B2E880D1}"/>
+    <hyperlink ref="J4" r:id="rId5" xr:uid="{15BF439D-4123-4A54-9B3D-42B9C4A470E3}"/>
+    <hyperlink ref="J8" r:id="rId6" xr:uid="{83C09D43-1C91-4DE0-AEBF-986F38CE3FF5}"/>
+    <hyperlink ref="J9" r:id="rId7" xr:uid="{E6D2BBE8-183F-4497-9029-7DBB5687D6D3}"/>
+    <hyperlink ref="J11" r:id="rId8" xr:uid="{552A9600-AAD6-462A-9E96-6A6C246201B3}"/>
+    <hyperlink ref="J12" r:id="rId9" xr:uid="{80DEF0DD-2E38-4B48-913C-4EF68FE67545}"/>
+    <hyperlink ref="J13" r:id="rId10" xr:uid="{4CB38AB4-C387-40E4-AC0E-7F7D05E0DFE3}"/>
+    <hyperlink ref="J14" r:id="rId11" xr:uid="{A7C867BB-0D09-46E4-90C2-91E7521767ED}"/>
+    <hyperlink ref="J15" r:id="rId12" xr:uid="{0177E209-49E6-4EF7-9CEF-661FB44C9B00}"/>
+    <hyperlink ref="J16" r:id="rId13" xr:uid="{4DC9186C-BD4B-4241-BD31-EF22D7C874CF}"/>
+    <hyperlink ref="J17" r:id="rId14" xr:uid="{788A3938-158B-40D2-ADEE-900398933E06}"/>
+    <hyperlink ref="J10" r:id="rId15" xr:uid="{AA7C1B3E-C812-42E3-BC04-2BBE7971EF28}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -876,7 +1050,7 @@
         <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -1103,7 +1277,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <v>70</v>
@@ -1132,7 +1306,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>75</v>
@@ -1161,7 +1335,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>80</v>
@@ -1190,7 +1364,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13">
         <v>85</v>

</xml_diff>

<commit_message>
update relifrsex by age
</commit_message>
<xml_diff>
--- a/data/deaths_location.xlsx
+++ b/data/deaths_location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan\Documents\GitHub\International-COVID-IFR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E698192E-64E4-4A47-8498-7AB054D9D590}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34631C4-E8B5-4023-BD40-A4BEEF78325C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7520" yWindow="1210" windowWidth="13640" windowHeight="9170" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0957DDB2-FF5A-4350-800D-AA3314930578}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update data & add 5 countries
</commit_message>
<xml_diff>
--- a/data/deaths_location.xlsx
+++ b/data/deaths_location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan\Documents\GitHub\International-COVID-IFR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34631C4-E8B5-4023-BD40-A4BEEF78325C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66F6B7F-CB4E-48CA-BB2D-CAD9C9ACAC37}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>country</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>pLTC</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>https://thl.fi/en/web/infectious-diseases/what-s-new/coronavirus-covid-19-latest-updates/situation-update-on-coronavirus#Coronavirus-related_deaths</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov/nchs/nvss/vsrr/covid_weekly/index.htm</t>
   </si>
 </sst>
 </file>
@@ -539,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0957DDB2-FF5A-4350-800D-AA3314930578}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,7 +657,7 @@
         <v>127</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I17" si="0">E3/C3</f>
+        <f t="shared" ref="I3:I19" si="0">E3/C3</f>
         <v>0.26056581804449758</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -732,21 +744,20 @@
         <v>43959</v>
       </c>
       <c r="C6">
-        <v>599</v>
+        <v>518</v>
       </c>
       <c r="D6">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="E6">
-        <f>269+5</f>
-        <v>274</v>
+        <v>184</v>
       </c>
       <c r="F6">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0.45742904841402338</v>
+        <v>0.35521235521235522</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>13</v>
@@ -993,6 +1004,57 @@
       </c>
       <c r="J17" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1">
+        <v>43979</v>
+      </c>
+      <c r="C18">
+        <v>313</v>
+      </c>
+      <c r="E18">
+        <v>141</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0.45047923322683708</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1">
+        <v>43974</v>
+      </c>
+      <c r="C19">
+        <v>81372</v>
+      </c>
+      <c r="D19">
+        <v>55903</v>
+      </c>
+      <c r="E19">
+        <v>20083</v>
+      </c>
+      <c r="F19">
+        <v>4247</v>
+      </c>
+      <c r="H19">
+        <v>1110</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0.24680479771911715</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1012,6 +1074,8 @@
     <hyperlink ref="J16" r:id="rId13" xr:uid="{4DC9186C-BD4B-4241-BD31-EF22D7C874CF}"/>
     <hyperlink ref="J17" r:id="rId14" xr:uid="{788A3938-158B-40D2-ADEE-900398933E06}"/>
     <hyperlink ref="J10" r:id="rId15" xr:uid="{AA7C1B3E-C812-42E3-BC04-2BBE7971EF28}"/>
+    <hyperlink ref="J18" r:id="rId16" location="Coronavirus-related_deaths" display="https://thl.fi/en/web/infectious-diseases/what-s-new/coronavirus-covid-19-latest-updates/situation-update-on-coronavirus - Coronavirus-related_deaths" xr:uid="{D858FE62-1458-4686-81F9-7AB74826A671}"/>
+    <hyperlink ref="J19" r:id="rId17" xr:uid="{1E1DE984-D198-4C79-87BF-33B572AFA380}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add Korea nursing home data
</commit_message>
<xml_diff>
--- a/data/deaths_location.xlsx
+++ b/data/deaths_location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan\Documents\GitHub\International-COVID-IFR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3C9D97-E472-4C48-B93F-8B7D1D128BE8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168373C0-FB59-469C-A94F-45C967AAA233}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="13060" windowHeight="9150" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
+    <workbookView xWindow="3610" yWindow="1770" windowWidth="13140" windowHeight="7740" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0957DDB2-FF5A-4350-800D-AA3314930578}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
add US and Korea adjusted data
</commit_message>
<xml_diff>
--- a/data/deaths_location.xlsx
+++ b/data/deaths_location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan\Documents\GitHub\International-COVID-IFR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168373C0-FB59-469C-A94F-45C967AAA233}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CA9E39-A7C8-486B-B0E6-0AD57B86D071}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3610" yWindow="1770" windowWidth="13140" windowHeight="7740" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
+    <workbookView xWindow="470" yWindow="1260" windowWidth="13140" windowHeight="7740" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>country</t>
   </si>
@@ -184,10 +184,13 @@
     <t>https://thl.fi/en/web/infectious-diseases/what-s-new/coronavirus-covid-19-latest-updates/situation-update-on-coronavirus#Coronavirus-related_deaths</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>https://www.cdc.gov/nchs/nvss/vsrr/covid_weekly/index.htm</t>
+  </si>
+  <si>
+    <t>Republic of Korea</t>
+  </si>
+  <si>
+    <t>United States of America</t>
   </si>
 </sst>
 </file>
@@ -551,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0957DDB2-FF5A-4350-800D-AA3314930578}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -657,7 +660,7 @@
         <v>127</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I19" si="0">E3/C3</f>
+        <f t="shared" ref="I3:I20" si="0">E3/C3</f>
         <v>0.26056581804449758</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1029,7 +1032,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1">
         <v>43974</v>
@@ -1054,7 +1057,22 @@
         <v>0.24680479771911715</v>
       </c>
       <c r="J19" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>51</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update functions & data
</commit_message>
<xml_diff>
--- a/data/deaths_location.xlsx
+++ b/data/deaths_location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan\Documents\GitHub\International-COVID-IFR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAF248C-A3A1-4E45-A01C-98C668DF3CFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBB0E08-F8F1-44B3-B9A4-336E2015A6BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
+    <workbookView xWindow="3350" yWindow="1490" windowWidth="7930" windowHeight="7550" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -611,26 +611,26 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>43961</v>
+        <v>44003</v>
       </c>
       <c r="C2">
-        <v>3213</v>
+        <v>4119</v>
       </c>
       <c r="D2">
-        <v>1537</v>
+        <v>1909</v>
       </c>
       <c r="E2">
-        <v>1438</v>
+        <v>1917</v>
       </c>
       <c r="F2">
-        <v>237</v>
+        <v>286</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I2">
         <f>E2/C2</f>
-        <v>0.44755680049797697</v>
+        <v>0.4654042243262928</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
update northern ireland data
</commit_message>
<xml_diff>
--- a/data/deaths_location.xlsx
+++ b/data/deaths_location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan\Documents\GitHub\International-COVID-IFR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC92DF62-2523-44B9-B2FF-89895CD040CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC630C7-5DE8-4E0B-896F-0015D1EDD8BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6470" yWindow="1290" windowWidth="11280" windowHeight="8950" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
+    <workbookView xWindow="450" yWindow="1770" windowWidth="11280" windowHeight="8950" xr2:uid="{715CC2EE-EC6E-482E-9097-D01DE953C3F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>country</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>https://www.cdc.gov/nchs/nvss/vsrr/covid_weekly/index.htm</t>
-  </si>
-  <si>
-    <t>Republic of Korea</t>
   </si>
   <si>
     <t>United States of America</t>
@@ -560,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0957DDB2-FF5A-4350-800D-AA3314930578}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -750,23 +747,26 @@
         <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>43959</v>
+        <v>44008</v>
       </c>
       <c r="C6">
-        <v>518</v>
+        <v>824</v>
       </c>
       <c r="D6">
-        <v>302</v>
+        <v>427</v>
       </c>
       <c r="E6">
-        <v>184</v>
+        <v>343</v>
       </c>
       <c r="F6">
-        <v>16</v>
+        <v>48</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0.35521235521235522</v>
+        <v>0.41626213592233008</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>13</v>
@@ -949,7 +949,7 @@
         <v>0.45733788395904434</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1038,7 +1038,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1">
         <v>43974</v>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1">
         <v>43988</v>
@@ -1099,7 +1099,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="1">
         <v>43988</v>
@@ -1126,21 +1126,6 @@
       </c>
       <c r="J21" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22">
-        <v>100</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>